<commit_message>
Added Github link to specification document
</commit_message>
<xml_diff>
--- a/Specification_doc__lockedMeApp.xlsx
+++ b/Specification_doc__lockedMeApp.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>LockedMeApp Specification Document</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>GitHub Link:</t>
+  </si>
+  <si>
+    <t>https://github.com/Priyam777/LockedMeApp_Priyadarshi_Panigrahi.git</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1078,7 @@
   <dimension ref="A1:C144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1154,12 +1157,17 @@
         <v>21</v>
       </c>
     </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="49" spans="1:3" s="5" customFormat="1">
       <c r="A49" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="2" customFormat="1" ht="60">
+    <row r="50" spans="1:3" s="2" customFormat="1" ht="30">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
@@ -1186,7 +1194,7 @@
     <row r="57" spans="1:3" s="2" customFormat="1">
       <c r="C57" s="3"/>
     </row>
-    <row r="59" spans="1:3" s="2" customFormat="1" ht="45">
+    <row r="59" spans="1:3" s="2" customFormat="1" ht="30">
       <c r="A59" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>